<commit_message>
Avance enorme en excel capataces, ya no hay datos duplicados, falta juntar las fechas
</commit_message>
<xml_diff>
--- a/target/classes/MEDICIONES BERLANGA-ANDALUZ DEL 18 AL 21 DE ABRIL.xlsx
+++ b/target/classes/MEDICIONES BERLANGA-ANDALUZ DEL 18 AL 21 DE ABRIL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\INES\Desktop\ROBERTO\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB6C03E-0C93-4A22-AD72-66629E47B779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DE561A-401A-4660-8402-8B3411BA156C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C66C163A-FC94-45BE-AEE2-81A12E3FD87B}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="50">
   <si>
     <t>DÍA</t>
   </si>
@@ -156,19 +156,52 @@
     <t>SERGIO</t>
   </si>
   <si>
-    <t>PRUEBAS</t>
-  </si>
-  <si>
-    <t>SADÑLNSA</t>
-  </si>
-  <si>
-    <t>GAM</t>
-  </si>
-  <si>
     <t>PEPE</t>
   </si>
   <si>
     <t>DAVID</t>
+  </si>
+  <si>
+    <t>UNO</t>
+  </si>
+  <si>
+    <t>DOS</t>
+  </si>
+  <si>
+    <t>TRES</t>
+  </si>
+  <si>
+    <t>CUATRO</t>
+  </si>
+  <si>
+    <t>CINCO</t>
+  </si>
+  <si>
+    <t>SEIS</t>
+  </si>
+  <si>
+    <t>SIETE</t>
+  </si>
+  <si>
+    <t>OCHO</t>
+  </si>
+  <si>
+    <t>NUEVE</t>
+  </si>
+  <si>
+    <t>DIEZ</t>
+  </si>
+  <si>
+    <t>ONCE</t>
+  </si>
+  <si>
+    <t>DOCE</t>
+  </si>
+  <si>
+    <t>TRECE</t>
+  </si>
+  <si>
+    <t>CATORCE</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1151,7 @@
   <dimension ref="B1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,9 +1235,11 @@
         <v>45037</v>
       </c>
       <c r="K5" s="36" t="s">
-        <v>38</v>
-      </c>
-      <c r="L5" s="37"/>
+        <v>35</v>
+      </c>
+      <c r="L5" s="37" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="38">
@@ -1228,7 +1263,7 @@
         <v>33</v>
       </c>
       <c r="L6" s="39" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1256,7 +1291,9 @@
       <c r="K7" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L7" s="39"/>
+      <c r="L7" s="39" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="8" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="38">
@@ -1279,7 +1316,9 @@
       <c r="K8" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L8" s="39"/>
+      <c r="L8" s="39" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="9" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="38">
@@ -1304,7 +1343,9 @@
       <c r="K9" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="39"/>
+      <c r="L9" s="39" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="38">
@@ -1331,7 +1372,9 @@
       <c r="K10" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L10" s="39"/>
+      <c r="L10" s="39" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="38">
@@ -1350,10 +1393,10 @@
         <v>44671</v>
       </c>
       <c r="K11" s="32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="L11" s="39" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1375,9 +1418,11 @@
         <v>44671</v>
       </c>
       <c r="K12" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="39"/>
+        <v>34</v>
+      </c>
+      <c r="L12" s="39" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="38">
@@ -1402,7 +1447,9 @@
       <c r="K13" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="39"/>
+      <c r="L13" s="39" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="14" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="38">
@@ -1424,7 +1471,7 @@
         <v>33</v>
       </c>
       <c r="L14" s="39" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1450,7 +1497,9 @@
       <c r="K15" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="39"/>
+      <c r="L15" s="39" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="16" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="38">
@@ -1471,7 +1520,9 @@
       <c r="K16" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="39"/>
+      <c r="L16" s="39" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="17" spans="2:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="38">
@@ -1496,7 +1547,9 @@
       <c r="K17" s="32" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="39"/>
+      <c r="L17" s="39" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="2:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="40">
@@ -1519,38 +1572,40 @@
       <c r="K18" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="43"/>
+      <c r="L18" s="43" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="19" spans="2:12" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="27" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="28">
-        <f>SUM(C5:C18)</f>
+        <f t="shared" ref="C19:I19" si="0">SUM(C5:C18)</f>
         <v>4422</v>
       </c>
       <c r="D19" s="28">
-        <f>SUM(D5:D18)</f>
+        <f t="shared" si="0"/>
         <v>101</v>
       </c>
       <c r="E19" s="28">
-        <f>SUM(E5:E18)</f>
+        <f t="shared" si="0"/>
         <v>44776</v>
       </c>
       <c r="F19" s="28">
-        <f>SUM(F5:F18)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="G19" s="28">
-        <f>SUM(G5:G18)</f>
+        <f t="shared" si="0"/>
         <v>868</v>
       </c>
       <c r="H19" s="28">
-        <f>SUM(H5:H18)</f>
+        <f t="shared" si="0"/>
         <v>1378</v>
       </c>
       <c r="I19" s="29">
-        <f>SUM(I5:I18)</f>
+        <f t="shared" si="0"/>
         <v>33</v>
       </c>
     </row>
@@ -1816,7 +1871,7 @@
       </c>
       <c r="I36" s="1"/>
       <c r="J36" s="1">
-        <f t="shared" ref="J36" si="0">F36*H36</f>
+        <f t="shared" ref="J36" si="1">F36*H36</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>